<commit_message>
adding the slide on recherche
</commit_message>
<xml_diff>
--- a/tables/Projets.xlsx
+++ b/tables/Projets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabio/Documents/Personal/MdC/Poste-ENSGSI/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24340B7-7F33-3243-8A46-C6279776B4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65C7047-9F2D-564F-AAF6-34E330D63A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{8BF84A60-ED26-7243-AAAF-D5A16B329311}"/>
   </bookViews>
@@ -115,9 +115,6 @@
     <t>Soumis Fev 2023</t>
   </si>
   <si>
-    <t xml:space="preserve">Participation au montage et à la coordination de du ERPI </t>
-  </si>
-  <si>
     <t>Creating Innovation and entrepreneurship ecosystems (U4BUSINESS)</t>
   </si>
   <si>
@@ -184,9 +181,6 @@
     <t>Participation au montage</t>
   </si>
   <si>
-    <t>Participation au montage et au Responsable scientifique</t>
-  </si>
-  <si>
     <t>EU HORIZON-RIA</t>
   </si>
   <si>
@@ -227,6 +221,12 @@
   </si>
   <si>
     <t>ÉValuation du rÉseau de REcyclage pour Soutenir la Transition vers une BIOéconomie (Everest Bio)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participation au montage et à la coordination ERPI </t>
+  </si>
+  <si>
+    <t>Participation au montage et  Responsable scientifique</t>
   </si>
 </sst>
 </file>
@@ -591,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2651365A-7D8C-954B-A69A-702ED2EF6AFC}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -620,7 +620,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>24</v>
@@ -631,19 +631,19 @@
         <v>2023</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="102" x14ac:dyDescent="0.2">
@@ -651,19 +651,19 @@
         <v>2023</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -671,19 +671,19 @@
         <v>2023</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="102" x14ac:dyDescent="0.2">
@@ -700,10 +700,10 @@
         <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -711,19 +711,19 @@
         <v>2022</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -731,19 +731,19 @@
         <v>2022</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="102" x14ac:dyDescent="0.2">
@@ -751,19 +751,19 @@
         <v>2021</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -777,13 +777,13 @@
         <v>13</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -794,16 +794,16 @@
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -823,7 +823,7 @@
         <v>20</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -843,7 +843,7 @@
         <v>11</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -863,7 +863,7 @@
         <v>21</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>